<commit_message>
Ajuste de codigo pyhon para evitar creacion de html, se agrego el banner como pie de pagina.
</commit_message>
<xml_diff>
--- a/jefatura.xlsx
+++ b/jefatura.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rodrigo.alexis\Desktop\mvp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE9B877-49A2-4E81-8A21-A2EFEEC03E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463D8FA0-0FA1-49E0-9628-D890B764D061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39330" yWindow="2430" windowWidth="14400" windowHeight="10035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="21">
   <si>
     <t>id_jefatura</t>
   </si>
@@ -60,23 +60,41 @@
     <t>U4</t>
   </si>
   <si>
-    <t>jefeclaro1@gmail.com</t>
-  </si>
-  <si>
     <t>jefeclaro2@gmail.com</t>
   </si>
   <si>
-    <t>Pablo Lobos</t>
-  </si>
-  <si>
-    <t>Martin Vidal</t>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>JEF-3</t>
+  </si>
+  <si>
+    <t>jefeclaro3@gmail.com</t>
+  </si>
+  <si>
+    <t>Gonzalo Lara</t>
+  </si>
+  <si>
+    <t>mariavyeguezp@gmail.com</t>
+  </si>
+  <si>
+    <t>ro.gonzalezl@duocuc.cl</t>
+  </si>
+  <si>
+    <t>Maria Yeguez</t>
+  </si>
+  <si>
+    <t>Rodrigo Gonzalez</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -94,6 +112,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -120,9 +146,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -404,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -415,7 +442,7 @@
     <col min="1" max="1" width="9.90625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.90625" customWidth="1"/>
-    <col min="4" max="4" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.54296875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -444,10 +471,10 @@
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -458,10 +485,10 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -472,10 +499,10 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -486,20 +513,54 @@
         <v>10</v>
       </c>
       <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="B6" t="s">
         <v>12</v>
       </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C9" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{B2916BBC-9936-4B4E-9EA6-895CCFD9E49A}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{909BA6C0-D164-4DA8-A7B6-F584F3C29271}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{DE704835-AAC2-4B6D-964C-30EFE2FDE1FD}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{49F93F8C-4116-40E2-B6E6-00527E6DB1DD}"/>
+    <hyperlink ref="D4" r:id="rId2" xr:uid="{DE704835-AAC2-4B6D-964C-30EFE2FDE1FD}"/>
+    <hyperlink ref="D5" r:id="rId3" xr:uid="{49F93F8C-4116-40E2-B6E6-00527E6DB1DD}"/>
+    <hyperlink ref="D6" r:id="rId4" xr:uid="{1C546C49-9BFC-4281-8BF9-16E8784C02BB}"/>
+    <hyperlink ref="D7" r:id="rId5" xr:uid="{77E6A904-F934-4879-A056-1339B71464A3}"/>
+    <hyperlink ref="D3" r:id="rId6" xr:uid="{D65495BD-63E2-45AB-BE21-8234D485C097}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>